<commit_message>
20250515 without elite inheritance
</commit_message>
<xml_diff>
--- a/results/MultiObjBaselines/communityStratifiedFMODGWO_facebook_final_pareto_solutions_detailed.xlsx
+++ b/results/MultiObjBaselines/communityStratifiedFMODGWO_facebook_final_pareto_solutions_detailed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,21 +478,21 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2483783114632335</v>
+        <v>0.2522901708343649</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7459890395576216</v>
+        <v>0.8817639482939641</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{896, 2369, 2347, 107, 2327, 3033, 2395, 2428, 414, 2334}</t>
+          <t>{641, 2631, 2183, 2601, 2986, 107, 2351, 1622, 2201, 2973}</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.131804227828979</v>
+        <v>2.352813243865967</v>
       </c>
       <c r="G2" t="n">
-        <v>1.401759113696259</v>
+        <v>0.5819225762028103</v>
       </c>
     </row>
     <row r="3">
@@ -503,21 +503,21 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2249319138400594</v>
+        <v>0.254518445159693</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8021240111910279</v>
+        <v>0.8273204540573542</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{1920, 2176, 1122, 2567, 107, 1420, 2323, 2740, 601, 1017}</t>
+          <t>{2273, 2183, 1320, 107, 2384, 3826, 2706, 2550, 3101, 2462}</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.131804227828979</v>
+        <v>2.352813243865967</v>
       </c>
       <c r="G3" t="n">
-        <v>1.401759113696259</v>
+        <v>0.5819225762028103</v>
       </c>
     </row>
     <row r="4">
@@ -528,321 +528,96 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2485763802921515</v>
+        <v>0.1631344392176281</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7130335701935486</v>
+        <v>0.9127066249820019</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{1192, 2601, 2410, 107, 3280, 2864, 1235, 1941, 2549, 2909}</t>
+          <t>{3907, 2244, 3366, 1001, 1515, 2348, 2292, 1049, 3101, 414}</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.131804227828979</v>
+        <v>2.352813243865967</v>
       </c>
       <c r="G4" t="n">
-        <v>1.401759113696259</v>
+        <v>0.5819225762028103</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
       <c r="C5" t="n">
-        <v>0.2396385243872245</v>
+        <v>0.2778905669720228</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7805161083104006</v>
+        <v>0.8756980904083504</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{1317, 2504, 2986, 107, 1322, 332, 1522, 2328, 2905, 2138}</t>
+          <t>{3201, 2694, 1864, 107, 3051, 109, 2353, 1076, 2038, 1912}</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.131804227828979</v>
+        <v>1.589942455291748</v>
       </c>
       <c r="G5" t="n">
-        <v>1.401759113696259</v>
+        <v>0.6327568357026606</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1579103738549146</v>
+        <v>0.2393414211438475</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8713653347757691</v>
+        <v>0.8962477314085928</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{2471, 1512, 1447, 590, 2606, 1680, 2414, 1235, 2132, 313}</t>
+          <t>{1447, 136, 1450, 107, 2090, 1486, 1616, 2706, 122, 2619}</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1.131804227828979</v>
+        <v>1.589942455291748</v>
       </c>
       <c r="G6" t="n">
-        <v>1.401759113696259</v>
+        <v>0.6327568357026606</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2088635800940827</v>
+        <v>0.1948502104481307</v>
       </c>
       <c r="D7" t="n">
-        <v>0.866067668714438</v>
+        <v>0.897609454607404</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{2240, 1793, 1701, 1800, 1001, 1962, 107, 269, 2866, 2556}</t>
+          <t>{0, 1536, 2500, 1126, 1577, 363, 3116, 1197, 239, 1758}</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1.131804227828979</v>
+        <v>1.589942455291748</v>
       </c>
       <c r="G7" t="n">
-        <v>1.401759113696259</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.2259965337954939</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.7875164350583255</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>{1730, 2564, 1158, 1479, 107, 236, 1391, 2607, 1625, 2138}</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1.131804227828979</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.401759113696259</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.21624164397128</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.8106657294381165</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>{2369, 484, 2118, 1799, 1703, 1767, 1459, 1684, 990, 1630}</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1.131804227828979</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1.401759113696259</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.2449863827680119</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.7627738433261086</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>{1185, 2273, 2053, 2469, 9, 2602, 107, 236, 2679, 1630}</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1.220318428865348</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.2383263183956425</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.7805161083104006</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>{896, 107, 1611, 2187, 1584, 2549, 213, 2392, 2333, 1630}</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1.220318428865348</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.2474622431294875</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.7465182257779897</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>{2560, 1786, 2469, 2631, 2344, 186, 107, 2125, 1146, 2877}</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1.220318428865348</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.2289923248328794</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.838139067920286</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>{1666, 2052, 2154, 107, 2475, 1838, 2484, 1881, 2649, 1211}</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1.220318428865348</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B14" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.1814310472889329</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.8455180277141956</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>{1273, 2123, 1613, 2253, 2578, 2679, 56, 2649, 1052, 1662}</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1.220318428865348</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B15" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.1463728645704382</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.8756980904083502</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>{3267, 1636, 3651, 2506, 2510, 2814, 2359, 1688, 156, 3038}</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1.220318428865348</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" t="n">
-        <v>7</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.235132458529339</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.8045998715525029</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>{1185, 67, 1509, 2153, 107, 2414, 2608, 213, 1078, 3032}</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>1.188111066818237</v>
-      </c>
-      <c r="G16" t="n">
-        <v>1.220318428865348</v>
+        <v>0.6327568357026606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>